<commit_message>
Added Director and Studio models with validations
</commit_message>
<xml_diff>
--- a/DB_structure.xlsx
+++ b/DB_structure.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Movies</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Limitation for Int are just 'to have' for exercising Data Notation Attributes</t>
+  </si>
+  <si>
+    <t>Trivia</t>
+  </si>
+  <si>
+    <t>Short Bio</t>
   </si>
 </sst>
 </file>
@@ -478,7 +484,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +535,9 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
@@ -546,6 +555,9 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
@@ -556,6 +568,9 @@
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>